<commit_message>
LV_Activities_Changes - 30 April 2024
</commit_message>
<xml_diff>
--- a/TestData/TMT0047429_VerifyActivityFunctionalityOnCompanyDetailPage.xlsx
+++ b/TestData/TMT0047429_VerifyActivityFunctionalityOnCompanyDetailPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90076F1-3207-4DF5-B31C-9952B6FB2B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22A1DF7-9DD9-417C-9B5D-E5B5503BB19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Module Name</t>
   </si>
   <si>
-    <t>FR Capital Provider</t>
-  </si>
-  <si>
     <t>Tab</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Updated Automated Test Subject Meeting</t>
+  </si>
+  <si>
+    <t>CapProviderTestCompany</t>
   </si>
 </sst>
 </file>
@@ -625,17 +625,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -658,32 +658,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95D2294-D185-4874-A4CE-34B75A6DBCF8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -711,7 +711,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +761,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,15 +787,15 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -819,13 +819,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +839,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +881,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -890,10 +890,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -913,10 +913,10 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -924,10 +924,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -936,10 +936,10 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -959,10 +959,10 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -992,24 +992,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1036,27 +1036,27 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1080,12 +1080,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1095,12 +1095,12 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -1115,7 +1115,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LV_Activities - 2nd May 2024
</commit_message>
<xml_diff>
--- a/TestData/TMT0047429_VerifyActivityFunctionalityOnCompanyDetailPage.xlsx
+++ b/TestData/TMT0047429_VerifyActivityFunctionalityOnCompanyDetailPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22A1DF7-9DD9-417C-9B5D-E5B5503BB19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCCB6EB-AFC2-418C-B96A-5243299F8CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>James Craven</t>
-  </si>
-  <si>
     <t>CompanyName</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>3 Months Ago</t>
   </si>
   <si>
-    <t>Please fill all of the required fields.</t>
-  </si>
-  <si>
     <t>The Activity has been saved successfully.</t>
   </si>
   <si>
@@ -242,6 +236,12 @@
   </si>
   <si>
     <t>CapProviderTestCompany</t>
+  </si>
+  <si>
+    <t>Indrajeet Singh</t>
+  </si>
+  <si>
+    <t>Complete this field.</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +601,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -625,17 +625,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -658,32 +658,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -706,12 +706,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -731,12 +731,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -756,12 +756,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -784,18 +784,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -819,13 +819,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -855,117 +855,117 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47E1313-6700-419E-B447-93C25ACEE135}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,24 +992,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1033,30 +1033,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1080,42 +1080,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LV_Activities - 26 June 2024
</commit_message>
<xml_diff>
--- a/TestData/TMT0047429_VerifyActivityFunctionalityOnCompanyDetailPage.xlsx
+++ b/TestData/TMT0047429_VerifyActivityFunctionalityOnCompanyDetailPage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB3D12B-7553-49D3-BB98-D237945B45BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1358887C-39AC-4435-AD27-77B765D46A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -235,13 +235,13 @@
     <t>Updated Automated Test Subject Meeting</t>
   </si>
   <si>
-    <t>CapProviderTestCompany</t>
-  </si>
-  <si>
     <t>Complete this field.</t>
   </si>
   <si>
-    <t>James Craven</t>
+    <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>ActivityCompany</t>
   </si>
 </sst>
 </file>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +601,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,7 +792,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>

</xml_diff>